<commit_message>
A bit more work on the BOM.
</commit_message>
<xml_diff>
--- a/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
+++ b/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FBD48B-0569-4D51-890F-4ACC64A69B99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2361D8E-2793-49C7-8A0F-E0996A38B6CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,20 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>STM32F102C8T6</t>
-  </si>
-  <si>
-    <t>MCU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>USB connector</t>
   </si>
   <si>
-    <t>14-pin debug header</t>
-  </si>
-  <si>
     <t>3.3V LDO</t>
   </si>
   <si>
@@ -43,7 +34,52 @@
     <t>Green LED</t>
   </si>
   <si>
-    <t>Target Power Switch</t>
+    <t>STM32F102CBU6</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>UFQFPN 48</t>
+  </si>
+  <si>
+    <t>DigiKey Part Number</t>
+  </si>
+  <si>
+    <t>497-17381-ND</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 128KB FLASH 48QFPN</t>
+  </si>
+  <si>
+    <t>609-3730-ND</t>
+  </si>
+  <si>
+    <t>20021121-00014T4LF</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD 14POS 1.27MM</t>
+  </si>
+  <si>
+    <t>CKN10722CT-ND</t>
+  </si>
+  <si>
+    <t>JS202011JAQN</t>
+  </si>
+  <si>
+    <t>Slide Switch DPDT Surface Mount, Right Angle</t>
   </si>
 </sst>
 </file>
@@ -361,53 +397,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:C10"/>
+  <dimension ref="A3:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>7</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on adapter board - got CPU in.
</commit_message>
<xml_diff>
--- a/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
+++ b/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCFCF17-0804-41E1-9439-1E5D23E7312A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82883758-D7CA-46C8-94EA-7B828AFC05AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>USB connector</t>
   </si>
   <si>
-    <t>3.3V LDO</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
     <t>Green LED</t>
   </si>
   <si>
-    <t>STM32F102CBU6</t>
-  </si>
-  <si>
     <t>Part Number</t>
   </si>
   <si>
@@ -119,6 +113,36 @@
   </si>
   <si>
     <t>3.3V target power LED</t>
+  </si>
+  <si>
+    <t>8MHz crystal</t>
+  </si>
+  <si>
+    <t>STM32F103CBU6</t>
+  </si>
+  <si>
+    <t>USB Reenumeration transistor</t>
+  </si>
+  <si>
+    <t>1727-4044-1-ND</t>
+  </si>
+  <si>
+    <t>TRANS NPN 40V 0.2A SOT23</t>
+  </si>
+  <si>
+    <t>MMBT3904,215</t>
+  </si>
+  <si>
+    <t>SOT23</t>
+  </si>
+  <si>
+    <t>497-3504-1-ND</t>
+  </si>
+  <si>
+    <t>LD3985M33R</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 150MA SOT23-5</t>
   </si>
 </sst>
 </file>
@@ -436,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,27 +471,27 @@
     <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -475,19 +499,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -503,16 +527,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -520,34 +544,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -555,16 +585,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -572,21 +602,21 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -594,7 +624,32 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adapter Board v2 done : set up for Larry and the EDT display
</commit_message>
<xml_diff>
--- a/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
+++ b/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82883758-D7CA-46C8-94EA-7B828AFC05AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CF6607-8F1D-4134-9464-415BA6D1632D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22725" yWindow="1995" windowWidth="20820" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>USB connector</t>
   </si>
@@ -143,6 +149,27 @@
   </si>
   <si>
     <t>IC REG LINEAR 3.3V 150MA SOT23-5</t>
+  </si>
+  <si>
+    <t>CRYSTAL 8.0000MHZ 12PF SMD</t>
+  </si>
+  <si>
+    <t>CX5032GB08000H0HPQZ1</t>
+  </si>
+  <si>
+    <t>1253-1373-2-ND</t>
+  </si>
+  <si>
+    <t>609-3714-ND</t>
+  </si>
+  <si>
+    <t>Through hole (across board edge) 2x7 debug header (must make boarod 0.8mm thick)</t>
+  </si>
+  <si>
+    <t>20021111-00014T4LF</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 14POS 1.27MM</t>
   </si>
 </sst>
 </file>
@@ -460,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:G16"/>
+  <dimension ref="A3:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +655,18 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
       <c r="G15" t="s">
         <v>31</v>
       </c>
@@ -650,6 +689,23 @@
       </c>
       <c r="G16" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM and ordered parts
</commit_message>
<xml_diff>
--- a/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
+++ b/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CF6607-8F1D-4134-9464-415BA6D1632D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1006661-790E-4F58-86A7-A022BD72A016}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22725" yWindow="1995" windowWidth="20820" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
-  <si>
-    <t>USB connector</t>
-  </si>
-  <si>
-    <t>Red LED</t>
-  </si>
-  <si>
-    <t>Green LED</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>Part Number</t>
   </si>
@@ -52,18 +43,9 @@
     <t>Package</t>
   </si>
   <si>
-    <t>UFQFPN 48</t>
-  </si>
-  <si>
     <t>DigiKey Part Number</t>
   </si>
   <si>
-    <t>497-17381-ND</t>
-  </si>
-  <si>
-    <t>IC MCU 32BIT 128KB FLASH 48QFPN</t>
-  </si>
-  <si>
     <t>609-3730-ND</t>
   </si>
   <si>
@@ -82,9 +64,6 @@
     <t>Slide Switch DPDT Surface Mount, Right Angle</t>
   </si>
   <si>
-    <t>Reset switch</t>
-  </si>
-  <si>
     <t>EG5384CT-ND</t>
   </si>
   <si>
@@ -112,9 +91,6 @@
     <t>4.7K resistor</t>
   </si>
   <si>
-    <t>Yellow LED</t>
-  </si>
-  <si>
     <t>ST-Link LED</t>
   </si>
   <si>
@@ -124,9 +100,6 @@
     <t>8MHz crystal</t>
   </si>
   <si>
-    <t>STM32F103CBU6</t>
-  </si>
-  <si>
     <t>USB Reenumeration transistor</t>
   </si>
   <si>
@@ -157,19 +130,220 @@
     <t>CX5032GB08000H0HPQZ1</t>
   </si>
   <si>
-    <t>1253-1373-2-ND</t>
-  </si>
-  <si>
     <t>609-3714-ND</t>
   </si>
   <si>
-    <t>Through hole (across board edge) 2x7 debug header (must make boarod 0.8mm thick)</t>
-  </si>
-  <si>
     <t>20021111-00014T4LF</t>
   </si>
   <si>
     <t>CONN HEADER VERT 14POS 1.27MM</t>
+  </si>
+  <si>
+    <t>497-17380-1-ND</t>
+  </si>
+  <si>
+    <t>48LQFP</t>
+  </si>
+  <si>
+    <t>STM32F103CBT6TR</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 128KB FLASH 48LQFP</t>
+  </si>
+  <si>
+    <t>H125270CT-ND</t>
+  </si>
+  <si>
+    <t>ZX62-B-5PA(33)</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
+  </si>
+  <si>
+    <t>USB MicroB</t>
+  </si>
+  <si>
+    <t>1253-1373-1-ND</t>
+  </si>
+  <si>
+    <t>Through hole (across board edge) 2x7 debug header (must make board 0.8mm thick)</t>
+  </si>
+  <si>
+    <t>Reset switch and boot switch</t>
+  </si>
+  <si>
+    <t>MMSD4148T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>SOD123</t>
+  </si>
+  <si>
+    <t>DIODE GEN PURP 100V 200MA SOD123</t>
+  </si>
+  <si>
+    <t>MMSD4148T1G</t>
+  </si>
+  <si>
+    <t>voltage measurement diode</t>
+  </si>
+  <si>
+    <t>R11,R12,R13,R14</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SW1,SW2</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>USB1</t>
+  </si>
+  <si>
+    <t>CN1</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>475-3124-1-ND</t>
+  </si>
+  <si>
+    <t>LS L29K-G1H2-1-Z</t>
+  </si>
+  <si>
+    <t>LED RED DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>475-3118-1-ND</t>
+  </si>
+  <si>
+    <t>LG L29K-F2J1-24-Z</t>
+  </si>
+  <si>
+    <t>LED GREEN DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>475-2794-1-ND</t>
+  </si>
+  <si>
+    <t>LY L29K-J1K2-26-Z</t>
+  </si>
+  <si>
+    <t>LED YELLOW DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>C11, C12</t>
+  </si>
+  <si>
+    <t>8MHz cyrstal load caps</t>
+  </si>
+  <si>
+    <t>311-1424-1-ND</t>
+  </si>
+  <si>
+    <t>SOD23-5</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>CC0603JRNPO9BN200</t>
+  </si>
+  <si>
+    <t>CAP CER 20PF 50V C0G/NPO 0603</t>
+  </si>
+  <si>
+    <t>C2,C5,C7,C8,C9,C10</t>
+  </si>
+  <si>
+    <t>22 ohm</t>
+  </si>
+  <si>
+    <t>C3,C6</t>
+  </si>
+  <si>
+    <t>1276-1182-1-ND</t>
+  </si>
+  <si>
+    <t>CL10A105KP8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 10V X5R 0603</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>399-17880-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C103K4RECAUTO</t>
+  </si>
+  <si>
+    <t>CAP CER 0603 10NF 16V X7R 10%</t>
+  </si>
+  <si>
+    <t>10 K ohm</t>
+  </si>
+  <si>
+    <t>100 ohm</t>
+  </si>
+  <si>
+    <t>1.5 K ohm</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>100K ohm</t>
+  </si>
+  <si>
+    <t>36K ohm</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>2.7K ohm</t>
+  </si>
+  <si>
+    <t>R22,R23</t>
+  </si>
+  <si>
+    <t>R9,R10</t>
+  </si>
+  <si>
+    <t>R2,R7,R8,R24,R21</t>
+  </si>
+  <si>
+    <t>R6,R17,R19,R1,R16</t>
+  </si>
+  <si>
+    <t>R4,R19,R20,R25,R26,R15</t>
+  </si>
+  <si>
+    <t>EasyLink v1</t>
   </si>
 </sst>
 </file>
@@ -205,8 +379,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:G18"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,211 +676,460 @@
     <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
         <v>35</v>
       </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="E33" t="s">
         <v>34</v>
       </c>
-      <c r="F16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="G33" t="s">
         <v>46</v>
-      </c>
-      <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added low profile switch option
</commit_message>
<xml_diff>
--- a/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
+++ b/board/EasyLink_v1/EasyLink_v1_BOM.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1006661-790E-4F58-86A7-A022BD72A016}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A201253-B9AE-47D6-8431-8513A24A3A1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
   <si>
     <t>Part Number</t>
   </si>
@@ -344,19 +343,31 @@
   </si>
   <si>
     <t>EasyLink v1</t>
+  </si>
+  <si>
+    <t>563-1102-1-ND</t>
+  </si>
+  <si>
+    <t>Low height (1.4mm) switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -379,9 +390,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1144,16 @@
         <v>46</v>
       </c>
     </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>